<commit_message>
gata sony, pias, nb
</commit_message>
<xml_diff>
--- a/Noutati/Mystic/MysticNoutati.xlsx
+++ b/Noutati/Mystic/MysticNoutati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei Bancila\Desktop\SupplierListManagerProject\Noutati\Mystic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A17C70D-519B-4A22-BC9D-137767CDED3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3B235C-417A-4021-8531-75B2C1518454}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3840" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6396" yWindow="2280" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Cod Bare</t>
   </si>
@@ -53,13 +53,19 @@
     <t>Pret PPD</t>
   </si>
   <si>
+    <t>Casa de discuri</t>
+  </si>
+  <si>
+    <t>Baracuda de pe lac</t>
+  </si>
+  <si>
+    <t>16 "Curves That Kick"</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
     <t>BY NORSE</t>
-  </si>
-  <si>
-    <t>16 "Curves That Kick"</t>
-  </si>
-  <si>
-    <t>CD</t>
   </si>
 </sst>
 </file>
@@ -403,13 +409,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,19 +437,22 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>7816770000000</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -454,8 +463,11 @@
       <c r="G2">
         <v>28.54</v>
       </c>
-      <c r="H2">
-        <f>IF(B2="Cooking_vinyl",G2*0.7*1.1,IF(B2="essential",G2*0.7*1.1,IF(B2="one Little Indian",G2*0.7*1.1,IF(B2="Season Of mist",G2*0.7*1.1,IF(B2="frontiers",G2*0.7*1.1,G2*0.75*1.1)))))</f>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2">
+        <f>IF(H2="Cooking_vinyl",G2*0.7*1.1,IF(H2="essential",G2*0.7*1.1,IF(H2="one Little Indian",G2*0.7*1.1,IF(H2="Season Of mist",G2*0.7*1.1,IF(H2="frontiers",G2*0.7*1.1,G2*0.75*1.1)))))</f>
         <v>23.545500000000004</v>
       </c>
     </row>

</xml_diff>

<commit_message>
gata cu piascls si cu mystic
</commit_message>
<xml_diff>
--- a/Noutati/Mystic/MysticNoutati.xlsx
+++ b/Noutati/Mystic/MysticNoutati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrei Bancila\Desktop\SupplierListManagerProject\Noutati\Mystic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3B235C-417A-4021-8531-75B2C1518454}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83065C23-581E-4CDA-9E12-D828E37E1462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6396" yWindow="2280" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12432" yWindow="4476" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>

</xml_diff>